<commit_message>
UI Additions in DetailedOutputLauout.axml
</commit_message>
<xml_diff>
--- a/TIPPER CALCULATIONS (APRIL 2017).xlsx
+++ b/TIPPER CALCULATIONS (APRIL 2017).xlsx
@@ -5652,8 +5652,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2608397" y="10339917"/>
-          <a:ext cx="10262259" cy="2490638"/>
+          <a:off x="2608397" y="17631833"/>
+          <a:ext cx="10262259" cy="2490639"/>
           <a:chOff x="4288866" y="20152331"/>
           <a:chExt cx="11520374" cy="2503671"/>
         </a:xfrm>
@@ -6248,8 +6248,8 @@
   </sheetPr>
   <dimension ref="A1:AF115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="65" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35:R35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="65" workbookViewId="0">
+      <selection activeCell="U17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7660,7 +7660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:32" ht="16.5" hidden="1" thickTop="1" thickBot="1">
+    <row r="49" spans="1:32" ht="16.5" thickTop="1" thickBot="1">
       <c r="A49" s="81"/>
       <c r="B49" s="423" t="s">
         <v>20</v>
@@ -7690,7 +7690,7 @@
       <c r="AC49" s="3"/>
       <c r="AF49" s="3"/>
     </row>
-    <row r="50" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="50" spans="1:32" ht="15.75" thickBot="1">
       <c r="A50" s="79"/>
       <c r="B50" s="362" t="s">
         <v>179</v>
@@ -7726,7 +7726,7 @@
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
     </row>
-    <row r="51" spans="1:32" hidden="1">
+    <row r="51" spans="1:32">
       <c r="A51" s="79"/>
       <c r="B51" s="428" t="s">
         <v>1</v>
@@ -7774,7 +7774,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
     </row>
-    <row r="52" spans="1:32" ht="18" hidden="1" thickBot="1">
+    <row r="52" spans="1:32" ht="18" thickBot="1">
       <c r="A52" s="79"/>
       <c r="B52" s="428" t="s">
         <v>2</v>
@@ -7813,7 +7813,7 @@
       </c>
       <c r="S52" s="80"/>
     </row>
-    <row r="53" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="53" spans="1:32" ht="15.75" thickBot="1">
       <c r="A53" s="79"/>
       <c r="B53" s="360" t="s">
         <v>3</v>
@@ -7849,7 +7849,7 @@
       </c>
       <c r="S53" s="80"/>
     </row>
-    <row r="54" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="54" spans="1:32" ht="15.75" thickBot="1">
       <c r="A54" s="79"/>
       <c r="B54" s="333" t="s">
         <v>4</v>
@@ -7885,7 +7885,7 @@
       </c>
       <c r="S54" s="80"/>
     </row>
-    <row r="55" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="55" spans="1:32" ht="15.75" thickBot="1">
       <c r="A55" s="79"/>
       <c r="B55" s="426" t="s">
         <v>0</v>
@@ -7913,7 +7913,7 @@
       <c r="R55" s="84"/>
       <c r="S55" s="80"/>
     </row>
-    <row r="56" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="56" spans="1:32" ht="15.75" thickBot="1">
       <c r="A56" s="79"/>
       <c r="B56" s="84"/>
       <c r="C56" s="84"/>
@@ -7934,7 +7934,7 @@
       <c r="R56" s="84"/>
       <c r="S56" s="80"/>
     </row>
-    <row r="57" spans="1:32" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="57" spans="1:32" ht="13.5" customHeight="1" thickBot="1">
       <c r="A57" s="79"/>
       <c r="B57" s="423" t="s">
         <v>21</v>
@@ -7959,7 +7959,7 @@
       <c r="R57" s="365"/>
       <c r="S57" s="80"/>
     </row>
-    <row r="58" spans="1:32" hidden="1">
+    <row r="58" spans="1:32">
       <c r="A58" s="79"/>
       <c r="B58" s="362" t="s">
         <v>0</v>
@@ -8000,7 +8000,7 @@
       </c>
       <c r="S58" s="80"/>
     </row>
-    <row r="59" spans="1:32" ht="18" hidden="1" thickBot="1">
+    <row r="59" spans="1:32" ht="18" thickBot="1">
       <c r="A59" s="79"/>
       <c r="B59" s="428" t="s">
         <v>8</v>
@@ -8042,7 +8042,7 @@
       </c>
       <c r="S59" s="80"/>
     </row>
-    <row r="60" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="60" spans="1:32" ht="15.75" thickBot="1">
       <c r="A60" s="79"/>
       <c r="B60" s="428" t="s">
         <v>9</v>
@@ -8072,7 +8072,7 @@
       <c r="R60" s="335"/>
       <c r="S60" s="80"/>
     </row>
-    <row r="61" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="61" spans="1:32" ht="15.75" thickBot="1">
       <c r="A61" s="79"/>
       <c r="B61" s="360" t="s">
         <v>10</v>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="S61" s="80"/>
     </row>
-    <row r="62" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="62" spans="1:32" ht="15.75" thickBot="1">
       <c r="A62" s="79"/>
       <c r="B62" s="387" t="s">
         <v>72</v>
@@ -8137,7 +8137,7 @@
       <c r="R62" s="335"/>
       <c r="S62" s="80"/>
     </row>
-    <row r="63" spans="1:32" ht="15.75" hidden="1" thickBot="1">
+    <row r="63" spans="1:32" ht="15.75" thickBot="1">
       <c r="A63" s="79"/>
       <c r="B63" s="384" t="s">
         <v>150</v>
@@ -8172,7 +8172,7 @@
       </c>
       <c r="S63" s="80"/>
     </row>
-    <row r="64" spans="1:32" hidden="1">
+    <row r="64" spans="1:32">
       <c r="A64" s="79"/>
       <c r="B64" s="381" t="s">
         <v>11</v>
@@ -8195,7 +8195,7 @@
       <c r="R64" s="84"/>
       <c r="S64" s="80"/>
     </row>
-    <row r="65" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="65" spans="1:22" ht="15.75" thickBot="1">
       <c r="A65" s="79"/>
       <c r="B65" s="407" t="s">
         <v>7</v>
@@ -8218,7 +8218,7 @@
       <c r="R65" s="84"/>
       <c r="S65" s="80"/>
     </row>
-    <row r="66" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="66" spans="1:22" ht="15.75" thickBot="1">
       <c r="A66" s="79"/>
       <c r="B66" s="392" t="s">
         <v>12</v>
@@ -8248,7 +8248,7 @@
       <c r="R66" s="365"/>
       <c r="S66" s="80"/>
     </row>
-    <row r="67" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="67" spans="1:22" ht="15.75" thickBot="1">
       <c r="A67" s="79"/>
       <c r="B67" s="390" t="s">
         <v>13</v>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="S67" s="80"/>
     </row>
-    <row r="68" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="68" spans="1:22" ht="15.75" thickBot="1">
       <c r="A68" s="79"/>
       <c r="B68" s="84"/>
       <c r="C68" s="84"/>
@@ -8322,7 +8322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="69" spans="1:22" ht="15.75" thickBot="1">
       <c r="A69" s="79"/>
       <c r="B69" s="363" t="s">
         <v>23</v>
@@ -8347,7 +8347,7 @@
       <c r="R69" s="335"/>
       <c r="S69" s="80"/>
     </row>
-    <row r="70" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="70" spans="1:22" ht="15.75" thickBot="1">
       <c r="A70" s="79"/>
       <c r="B70" s="378" t="s">
         <v>185</v>
@@ -8387,7 +8387,7 @@
       </c>
       <c r="S70" s="80"/>
     </row>
-    <row r="71" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="71" spans="1:22" ht="15.75" thickBot="1">
       <c r="A71" s="79"/>
       <c r="B71" s="378" t="s">
         <v>186</v>
@@ -8418,7 +8418,7 @@
       <c r="S71" s="80"/>
       <c r="U71" s="21"/>
     </row>
-    <row r="72" spans="1:22" ht="18" hidden="1" thickBot="1">
+    <row r="72" spans="1:22" ht="18" thickBot="1">
       <c r="A72" s="79"/>
       <c r="B72" s="378" t="s">
         <v>187</v>
@@ -8458,7 +8458,7 @@
       </c>
       <c r="S72" s="80"/>
     </row>
-    <row r="73" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="73" spans="1:22" ht="15.75" thickBot="1">
       <c r="A73" s="79"/>
       <c r="B73" s="489" t="s">
         <v>17</v>
@@ -8486,7 +8486,7 @@
       <c r="R73" s="84"/>
       <c r="S73" s="80"/>
     </row>
-    <row r="74" spans="1:22" ht="16.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="74" spans="1:22" ht="16.5" customHeight="1" thickBot="1">
       <c r="A74" s="79"/>
       <c r="B74" s="333" t="s">
         <v>16</v>
@@ -8510,7 +8510,7 @@
       <c r="S74" s="80"/>
       <c r="T74" s="30"/>
     </row>
-    <row r="75" spans="1:22" ht="15.75" hidden="1" customHeight="1" thickBot="1">
+    <row r="75" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A75" s="79"/>
       <c r="B75" s="60" t="s">
         <v>32</v>
@@ -8546,7 +8546,7 @@
       <c r="S75" s="80"/>
       <c r="T75" s="30"/>
     </row>
-    <row r="76" spans="1:22" ht="16.5" hidden="1" thickBot="1">
+    <row r="76" spans="1:22" ht="16.5" thickBot="1">
       <c r="A76" s="79"/>
       <c r="B76" s="84"/>
       <c r="C76" s="84"/>
@@ -8574,7 +8574,7 @@
       <c r="S76" s="80"/>
       <c r="T76" s="30"/>
     </row>
-    <row r="77" spans="1:22" ht="15.75" hidden="1" thickBot="1">
+    <row r="77" spans="1:22" ht="15.75" thickBot="1">
       <c r="A77" s="79"/>
       <c r="B77" s="267" t="s">
         <v>50</v>
@@ -8604,7 +8604,7 @@
       <c r="R77" s="121"/>
       <c r="S77" s="80"/>
     </row>
-    <row r="78" spans="1:22" ht="15.75" hidden="1" customHeight="1">
+    <row r="78" spans="1:22" ht="15.75" customHeight="1">
       <c r="A78" s="79"/>
       <c r="B78" s="362" t="s">
         <v>185</v>
@@ -8649,7 +8649,7 @@
       <c r="U78" s="10"/>
       <c r="V78" s="259"/>
     </row>
-    <row r="79" spans="1:22" ht="15.75" hidden="1" customHeight="1" thickBot="1">
+    <row r="79" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A79" s="79"/>
       <c r="B79" s="428" t="s">
         <v>186</v>
@@ -8687,7 +8687,7 @@
       <c r="U79" s="10"/>
       <c r="V79" s="259"/>
     </row>
-    <row r="80" spans="1:22" ht="15.75" hidden="1" customHeight="1" thickBot="1">
+    <row r="80" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A80" s="79"/>
       <c r="B80" s="360" t="s">
         <v>187</v>
@@ -8731,7 +8731,7 @@
       <c r="U80" s="10"/>
       <c r="V80" s="259"/>
     </row>
-    <row r="81" spans="1:19" ht="15.75" hidden="1" thickBot="1">
+    <row r="81" spans="1:19" ht="15.75" thickBot="1">
       <c r="A81" s="79"/>
       <c r="B81" s="271" t="s">
         <v>33</v>
@@ -8761,7 +8761,7 @@
       <c r="R81" s="121"/>
       <c r="S81" s="80"/>
     </row>
-    <row r="82" spans="1:19" ht="15.75" hidden="1" customHeight="1">
+    <row r="82" spans="1:19" ht="15.75" customHeight="1">
       <c r="A82" s="79"/>
       <c r="B82" s="494" t="s">
         <v>195</v>
@@ -8798,7 +8798,7 @@
       <c r="R82" s="538"/>
       <c r="S82" s="80"/>
     </row>
-    <row r="83" spans="1:19" ht="15.75" hidden="1" thickBot="1">
+    <row r="83" spans="1:19" ht="15.75" thickBot="1">
       <c r="A83" s="79"/>
       <c r="B83" s="496"/>
       <c r="C83" s="497"/>
@@ -8833,7 +8833,7 @@
       </c>
       <c r="S83" s="80"/>
     </row>
-    <row r="84" spans="1:19" ht="15.75" hidden="1" thickBot="1">
+    <row r="84" spans="1:19" ht="15.75" thickBot="1">
       <c r="A84" s="79"/>
       <c r="B84" s="84"/>
       <c r="C84" s="84"/>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="S84" s="80"/>
     </row>
-    <row r="85" spans="1:19" ht="16.5" thickTop="1" thickBot="1">
+    <row r="85" spans="1:19" ht="15.75" thickBot="1">
       <c r="A85" s="86"/>
       <c r="B85" s="87"/>
       <c r="C85" s="87"/>
@@ -9502,7 +9502,7 @@
   </sheetPr>
   <dimension ref="A1:AO93"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA39" sqref="AA39"/>
     </sheetView>
   </sheetViews>

</xml_diff>